<commit_message>
Travail du week-end, heuristique4000 pas finie + ajout d'autres trucs...
</commit_message>
<xml_diff>
--- a/instances/solutions.xlsx
+++ b/instances/solutions.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="18720" windowHeight="13460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Distances dépôt – client identique pour tous les clients</t>
   </si>
@@ -77,13 +82,19 @@
   </si>
   <si>
     <t>Instance20n4cl-h</t>
+  </si>
+  <si>
+    <t>pas attendu la fin de la recherche à partir de là</t>
+  </si>
+  <si>
+    <t>Djamel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,13 +102,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -112,8 +141,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -174,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -209,7 +241,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -418,26 +450,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F3" sqref="F3:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -447,8 +480,11 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -461,8 +497,11 @@
       <c r="D4">
         <v>731.09604146020104</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -475,8 +514,11 @@
       <c r="D5">
         <v>1874.2573467433299</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -489,8 +531,14 @@
       <c r="D6">
         <v>2306.2401001911799</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>2754</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -503,8 +551,14 @@
       <c r="D7">
         <v>1439.9720490007201</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>3827</v>
+      </c>
+      <c r="F7">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -517,8 +571,14 @@
       <c r="D8">
         <v>1405.2140481199301</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>1965</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -531,8 +591,14 @@
       <c r="D9">
         <v>3082.7755786605999</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>5921</v>
+      </c>
+      <c r="F9">
+        <v>5175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -545,8 +611,14 @@
       <c r="D10">
         <v>2792.2614076611799</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>5654</v>
+      </c>
+      <c r="F10">
+        <v>4947</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -559,13 +631,19 @@
       <c r="D11">
         <v>2595.45794626222</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>5070</v>
+      </c>
+      <c r="F11">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="B16" t="s">
         <v>1</v>
       </c>
@@ -576,7 +654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -589,8 +667,11 @@
       <c r="D17">
         <v>673.78196239762497</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -603,8 +684,11 @@
       <c r="D18">
         <v>1687.26868340699</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -617,8 +701,11 @@
       <c r="D19">
         <v>2582.8993009156302</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1">
+        <v>2985</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -631,8 +718,14 @@
       <c r="D20">
         <v>1331.58145410063</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1">
+        <v>3707</v>
+      </c>
+      <c r="F20">
+        <v>3432</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -645,8 +738,14 @@
       <c r="D21">
         <v>1476.0140481221299</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1">
+        <v>2106</v>
+      </c>
+      <c r="F21" s="3">
+        <v>3478</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -659,8 +758,14 @@
       <c r="D22">
         <v>3306.7605499715401</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1">
+        <v>5921</v>
+      </c>
+      <c r="F22">
+        <v>4934</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -673,8 +778,14 @@
       <c r="D23">
         <v>3300.9120289893299</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <v>5972</v>
+      </c>
+      <c r="F23">
+        <v>5109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -687,8 +798,19 @@
       <c r="D24">
         <v>2384.8324099708302</v>
       </c>
+      <c r="E24" s="1">
+        <v>5439</v>
+      </c>
+      <c r="F24">
+        <v>5079</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Màj stats. On bat Pool partout... Mon tri ne s'avère pas si bon :c
</commit_message>
<xml_diff>
--- a/instances/solutions.xlsx
+++ b/instances/solutions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="18720" windowHeight="13460"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="25300" windowHeight="16580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Distances dépôt – client identique pour tous les clients</t>
   </si>
@@ -84,17 +84,20 @@
     <t>Instance20n4cl-h</t>
   </si>
   <si>
-    <t>pas attendu la fin de la recherche à partir de là</t>
-  </si>
-  <si>
     <t>Djamel</t>
+  </si>
+  <si>
+    <t>Tri 2 blk</t>
+  </si>
+  <si>
+    <t>Tps de calcul, Tri 1 indo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,8 +117,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +134,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,11 +156,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -463,14 +480,15 @@
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
     <col min="5" max="5" width="7.5" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -481,10 +499,16 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -500,8 +524,14 @@
       <c r="E4" s="1">
         <v>1211</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" s="4">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5.17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -517,8 +547,14 @@
       <c r="E5" s="2">
         <v>1874</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="4">
+        <v>16.14</v>
+      </c>
+      <c r="H5" s="4">
+        <v>16.14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -534,11 +570,14 @@
       <c r="E6" s="1">
         <v>2606</v>
       </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="5">
+        <v>2606</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2754</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -557,8 +596,14 @@
       <c r="F7">
         <v>3461</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="5">
+        <v>1999</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -577,8 +622,14 @@
       <c r="F8" s="3">
         <v>3127</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" s="5">
+        <v>1965</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -597,8 +648,14 @@
       <c r="F9">
         <v>5175</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" s="5">
+        <v>4736</v>
+      </c>
+      <c r="H9" s="5">
+        <v>4736</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -617,8 +674,14 @@
       <c r="F10">
         <v>4947</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10" s="5">
+        <v>3937</v>
+      </c>
+      <c r="H10" s="5">
+        <v>3937</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -637,13 +700,19 @@
       <c r="F11">
         <v>4761</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="G11" s="5">
+        <v>4142</v>
+      </c>
+      <c r="H11" s="5">
+        <v>4142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="B16" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Ajout de critères de tris. Tests
</commit_message>
<xml_diff>
--- a/instances/solutions.xlsx
+++ b/instances/solutions.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -593,7 +593,7 @@
       <c r="E7" s="1">
         <v>3827</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>3461</v>
       </c>
       <c r="G7" s="5">
@@ -645,7 +645,7 @@
       <c r="E9" s="1">
         <v>5921</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>5175</v>
       </c>
       <c r="G9" s="5">
@@ -671,7 +671,7 @@
       <c r="E10" s="1">
         <v>5654</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>4947</v>
       </c>
       <c r="G10" s="5">
@@ -697,7 +697,7 @@
       <c r="E11" s="1">
         <v>5070</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>4761</v>
       </c>
       <c r="G11" s="5">

</xml_diff>